<commit_message>
1st Prod version / Updated CC email field
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\AUS-SRV-FS01\RedirectedFolders$\svc_rpabot_dev02\Documents\UiPath\Legal_DropList_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC850116-77BB-4A29-B693-3A63E39077D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD21CDE9-C758-4795-8EE2-AB976330BCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="26160" windowHeight="15705" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -181,9 +181,6 @@
     <t>EmailAccount</t>
   </si>
   <si>
-    <t>13_EmailAddressDev02</t>
-  </si>
-  <si>
     <t>Email account in which the DropList report is being sent to</t>
   </si>
   <si>
@@ -260,6 +257,18 @@
   </si>
   <si>
     <t>Remarks</t>
+  </si>
+  <si>
+    <t>13_EmailAddress</t>
+  </si>
+  <si>
+    <t>CCEmail</t>
+  </si>
+  <si>
+    <t>13_CCEmail</t>
+  </si>
+  <si>
+    <t>Tech email account</t>
   </si>
 </sst>
 </file>
@@ -542,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2813,7 +2822,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2862,100 +2873,113 @@
         <v>51</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="10" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3972,25 +3996,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated write row actions
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\AUS-SRV-FS01\RedirectedFolders$\svc_rpabot_dev02\Documents\UiPath\Legal_DropList_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD21CDE9-C758-4795-8EE2-AB976330BCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755785BA-01A2-40A9-8002-29E834A79C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="26160" windowHeight="15705" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="10695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -193,9 +193,6 @@
     <t>GDrive folder path where the execution reports are stored</t>
   </si>
   <si>
-    <t>GDriveMasterReport</t>
-  </si>
-  <si>
     <t>13_GDriveMasterReportPath</t>
   </si>
   <si>
@@ -269,6 +266,18 @@
   </si>
   <si>
     <t>Tech email account</t>
+  </si>
+  <si>
+    <t>13_GDriveMasterReportID</t>
+  </si>
+  <si>
+    <t>GDriveMasterReportPath</t>
+  </si>
+  <si>
+    <t>GDriveMasterReportID</t>
+  </si>
+  <si>
+    <t>Gdrive file ID for the Master execution report</t>
   </si>
 </sst>
 </file>
@@ -2823,7 +2832,7 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2873,7 +2882,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
@@ -2898,89 +2907,102 @@
     </row>
     <row r="4" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
         <v>81</v>
       </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3996,25 +4018,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated logic to retry write row actions / Added module to update Lead Sheet
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\AUS-SRV-FS01\RedirectedFolders$\svc_rpabot_dev02\Documents\UiPath\Legal_DropList_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755785BA-01A2-40A9-8002-29E834A79C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C92176-B03B-4003-974B-310C5FDD62B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="10695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4980" yWindow="3390" windowWidth="21600" windowHeight="10695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -278,6 +278,15 @@
   </si>
   <si>
     <t>Gdrive file ID for the Master execution report</t>
+  </si>
+  <si>
+    <t>13_LeadSheetID</t>
+  </si>
+  <si>
+    <t>LeadSheetID</t>
+  </si>
+  <si>
+    <t>Gdrive file ID for the Lead Spreadsheet document</t>
   </si>
 </sst>
 </file>
@@ -2832,7 +2841,7 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3003,7 +3012,20 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
     <row r="12" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented logic to re utilize report file and remove blank spaces from Lead spreadsheet
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\AUS-SRV-FS01\RedirectedFolders$\svc_rpabot_dev02\Documents\UiPath\Legal_DropList_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C92176-B03B-4003-974B-310C5FDD62B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4B0893-61FF-4032-9F7C-4300AC308CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="3390" windowWidth="21600" windowHeight="10695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="10695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -287,6 +287,33 @@
   </si>
   <si>
     <t>Gdrive file ID for the Lead Spreadsheet document</t>
+  </si>
+  <si>
+    <t>Gdrive file URL for the Lead Spreadsheet document</t>
+  </si>
+  <si>
+    <t>13_LeadSheetURL</t>
+  </si>
+  <si>
+    <t>LeadSheetURL</t>
+  </si>
+  <si>
+    <t>ReportFileID</t>
+  </si>
+  <si>
+    <t>ReportFileURL</t>
+  </si>
+  <si>
+    <t>13_ReportFileID</t>
+  </si>
+  <si>
+    <t>13_ReportFileURL</t>
+  </si>
+  <si>
+    <t>Gdrive file ID for the current execution report</t>
+  </si>
+  <si>
+    <t>Gdrive file URL for the current execution report</t>
   </si>
 </sst>
 </file>
@@ -2841,7 +2868,7 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3026,9 +3053,48 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
     <row r="15" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>